<commit_message>
1. Make gender optionl 2. Generate teacher collection 3. dynamic caculate price
</commit_message>
<xml_diff>
--- a/data-transfer/transfer/data/cca/cca-class.xlsx
+++ b/data-transfer/transfer/data/cca/cca-class.xlsx
@@ -402,7 +402,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -412,8 +412,14 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,7 +577,13 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -670,10 +682,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
+            <a:latin typeface="Cambria"/>
+            <a:ea typeface="Cambria"/>
+            <a:cs typeface="Cambria"/>
+            <a:sym typeface="Cambria"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -928,7 +940,13 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1241,10 +1259,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
+            <a:latin typeface="Cambria"/>
+            <a:ea typeface="Cambria"/>
+            <a:cs typeface="Cambria"/>
+            <a:sym typeface="Cambria"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1498,7 +1516,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1512,7 +1530,9 @@
     <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
-    <col min="9" max="256" width="14.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="1" customWidth="1"/>
+    <col min="11" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
@@ -1540,6 +1560,8 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" ht="17" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1554,7 +1576,7 @@
       <c r="D2" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="4">
         <v>12</v>
       </c>
       <c r="F2" t="s" s="2">
@@ -1566,6 +1588,8 @@
       <c r="H2" t="s" s="2">
         <v>15</v>
       </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" ht="17" customHeight="1">
       <c r="A3" t="s" s="2">
@@ -1580,7 +1604,7 @@
       <c r="D3" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="3">
+      <c r="E3" t="s" s="4">
         <v>17</v>
       </c>
       <c r="F3" t="s" s="2">
@@ -1592,6 +1616,8 @@
       <c r="H3" t="s" s="2">
         <v>18</v>
       </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" ht="17" customHeight="1">
       <c r="A4" t="s" s="2">
@@ -1606,7 +1632,7 @@
       <c r="D4" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="E4" t="s" s="3">
+      <c r="E4" t="s" s="4">
         <v>20</v>
       </c>
       <c r="F4" t="s" s="2">
@@ -1618,6 +1644,8 @@
       <c r="H4" t="s" s="2">
         <v>21</v>
       </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" ht="17" customHeight="1">
       <c r="A5" t="s" s="2">
@@ -1632,7 +1660,7 @@
       <c r="D5" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E5" t="s" s="3">
+      <c r="E5" t="s" s="4">
         <v>24</v>
       </c>
       <c r="F5" t="s" s="2">
@@ -1644,6 +1672,8 @@
       <c r="H5" t="s" s="2">
         <v>25</v>
       </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" ht="17" customHeight="1">
       <c r="A6" t="s" s="2">
@@ -1658,7 +1688,7 @@
       <c r="D6" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E6" t="s" s="3">
+      <c r="E6" t="s" s="4">
         <v>26</v>
       </c>
       <c r="F6" t="s" s="2">
@@ -1670,6 +1700,8 @@
       <c r="H6" t="s" s="2">
         <v>27</v>
       </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" ht="17" customHeight="1">
       <c r="A7" t="s" s="2">
@@ -1684,7 +1716,7 @@
       <c r="D7" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E7" t="s" s="3">
+      <c r="E7" t="s" s="4">
         <v>28</v>
       </c>
       <c r="F7" t="s" s="2">
@@ -1696,6 +1728,8 @@
       <c r="H7" t="s" s="2">
         <v>29</v>
       </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" t="s" s="2">
@@ -1710,7 +1744,7 @@
       <c r="D8" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E8" t="s" s="3">
+      <c r="E8" t="s" s="4">
         <v>30</v>
       </c>
       <c r="F8" t="s" s="2">
@@ -1722,6 +1756,8 @@
       <c r="H8" t="s" s="2">
         <v>31</v>
       </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" t="s" s="2">
@@ -1736,7 +1772,7 @@
       <c r="D9" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E9" t="s" s="3">
+      <c r="E9" t="s" s="4">
         <v>32</v>
       </c>
       <c r="F9" t="s" s="2">
@@ -1748,6 +1784,8 @@
       <c r="H9" t="s" s="2">
         <v>33</v>
       </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" t="s" s="2">
@@ -1762,7 +1800,7 @@
       <c r="D10" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E10" t="s" s="3">
+      <c r="E10" t="s" s="4">
         <v>34</v>
       </c>
       <c r="F10" t="s" s="2">
@@ -1774,6 +1812,8 @@
       <c r="H10" t="s" s="2">
         <v>35</v>
       </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" ht="17" customHeight="1">
       <c r="A11" t="s" s="2">
@@ -1788,7 +1828,7 @@
       <c r="D11" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E11" t="s" s="3">
+      <c r="E11" t="s" s="4">
         <v>17</v>
       </c>
       <c r="F11" t="s" s="2">
@@ -1800,6 +1840,8 @@
       <c r="H11" t="s" s="2">
         <v>36</v>
       </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" ht="17" customHeight="1">
       <c r="A12" t="s" s="2">
@@ -1814,7 +1856,7 @@
       <c r="D12" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="E12" t="s" s="3">
+      <c r="E12" t="s" s="4">
         <v>20</v>
       </c>
       <c r="F12" t="s" s="2">
@@ -1826,6 +1868,8 @@
       <c r="H12" t="s" s="2">
         <v>38</v>
       </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" ht="17" customHeight="1">
       <c r="A13" t="s" s="2">
@@ -1840,7 +1884,7 @@
       <c r="D13" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="E13" t="s" s="3">
+      <c r="E13" t="s" s="4">
         <v>40</v>
       </c>
       <c r="F13" t="s" s="2">
@@ -1852,6 +1896,8 @@
       <c r="H13" t="s" s="2">
         <v>41</v>
       </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" ht="17" customHeight="1">
       <c r="A14" t="s" s="2">
@@ -1866,7 +1912,7 @@
       <c r="D14" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E14" t="s" s="3">
+      <c r="E14" t="s" s="4">
         <v>24</v>
       </c>
       <c r="F14" t="s" s="2">
@@ -1878,6 +1924,8 @@
       <c r="H14" t="s" s="2">
         <v>43</v>
       </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" ht="17" customHeight="1">
       <c r="A15" t="s" s="2">
@@ -1892,7 +1940,7 @@
       <c r="D15" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E15" t="s" s="3">
+      <c r="E15" t="s" s="4">
         <v>26</v>
       </c>
       <c r="F15" t="s" s="2">
@@ -1904,6 +1952,8 @@
       <c r="H15" t="s" s="2">
         <v>44</v>
       </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" ht="17" customHeight="1">
       <c r="A16" t="s" s="2">
@@ -1918,7 +1968,7 @@
       <c r="D16" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E16" t="s" s="3">
+      <c r="E16" t="s" s="4">
         <v>28</v>
       </c>
       <c r="F16" t="s" s="2">
@@ -1930,6 +1980,8 @@
       <c r="H16" t="s" s="2">
         <v>45</v>
       </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" ht="17" customHeight="1">
       <c r="A17" t="s" s="2">
@@ -1944,7 +1996,7 @@
       <c r="D17" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E17" t="s" s="3">
+      <c r="E17" t="s" s="4">
         <v>30</v>
       </c>
       <c r="F17" t="s" s="2">
@@ -1956,6 +2008,8 @@
       <c r="H17" t="s" s="2">
         <v>46</v>
       </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
     </row>
     <row r="18" ht="17" customHeight="1">
       <c r="A18" t="s" s="2">
@@ -1970,7 +2024,7 @@
       <c r="D18" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E18" t="s" s="3">
+      <c r="E18" t="s" s="4">
         <v>32</v>
       </c>
       <c r="F18" t="s" s="2">
@@ -1982,6 +2036,8 @@
       <c r="H18" t="s" s="2">
         <v>47</v>
       </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" ht="17" customHeight="1">
       <c r="A19" t="s" s="2">
@@ -1996,7 +2052,7 @@
       <c r="D19" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E19" t="s" s="3">
+      <c r="E19" t="s" s="4">
         <v>48</v>
       </c>
       <c r="F19" t="s" s="2">
@@ -2008,6 +2064,8 @@
       <c r="H19" t="s" s="2">
         <v>49</v>
       </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
     </row>
     <row r="20" ht="17" customHeight="1">
       <c r="A20" t="s" s="2">
@@ -2022,7 +2080,7 @@
       <c r="D20" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E20" t="s" s="3">
+      <c r="E20" t="s" s="4">
         <v>52</v>
       </c>
       <c r="F20" t="s" s="2">
@@ -2034,6 +2092,8 @@
       <c r="H20" t="s" s="2">
         <v>54</v>
       </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
     </row>
     <row r="21" ht="17" customHeight="1">
       <c r="A21" t="s" s="2">
@@ -2048,7 +2108,7 @@
       <c r="D21" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E21" t="s" s="3">
+      <c r="E21" t="s" s="4">
         <v>57</v>
       </c>
       <c r="F21" t="s" s="2">
@@ -2060,6 +2120,8 @@
       <c r="H21" t="s" s="2">
         <v>59</v>
       </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
     </row>
     <row r="22" ht="17" customHeight="1">
       <c r="A22" t="s" s="2">
@@ -2074,7 +2136,7 @@
       <c r="D22" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E22" t="s" s="3">
+      <c r="E22" t="s" s="4">
         <v>12</v>
       </c>
       <c r="F22" t="s" s="2">
@@ -2086,6 +2148,8 @@
       <c r="H22" t="s" s="2">
         <v>60</v>
       </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
     </row>
     <row r="23" ht="17" customHeight="1">
       <c r="A23" t="s" s="2">
@@ -2100,7 +2164,7 @@
       <c r="D23" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E23" t="s" s="3">
+      <c r="E23" t="s" s="4">
         <v>61</v>
       </c>
       <c r="F23" t="s" s="2">
@@ -2112,6 +2176,8 @@
       <c r="H23" t="s" s="2">
         <v>62</v>
       </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
     </row>
     <row r="24" ht="17" customHeight="1">
       <c r="A24" t="s" s="2">
@@ -2126,7 +2192,7 @@
       <c r="D24" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="E24" t="s" s="3">
+      <c r="E24" t="s" s="4">
         <v>63</v>
       </c>
       <c r="F24" t="s" s="2">
@@ -2138,6 +2204,8 @@
       <c r="H24" t="s" s="2">
         <v>64</v>
       </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
     </row>
     <row r="25" ht="17" customHeight="1">
       <c r="A25" t="s" s="2">
@@ -2152,7 +2220,7 @@
       <c r="D25" t="s" s="2">
         <v>65</v>
       </c>
-      <c r="E25" t="s" s="3">
+      <c r="E25" t="s" s="4">
         <v>20</v>
       </c>
       <c r="F25" t="s" s="2">
@@ -2164,6 +2232,8 @@
       <c r="H25" t="s" s="2">
         <v>66</v>
       </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
     </row>
     <row r="26" ht="17" customHeight="1">
       <c r="A26" t="s" s="2">
@@ -2178,7 +2248,7 @@
       <c r="D26" t="s" s="2">
         <v>65</v>
       </c>
-      <c r="E26" t="s" s="3">
+      <c r="E26" t="s" s="4">
         <v>20</v>
       </c>
       <c r="F26" t="s" s="2">
@@ -2190,6 +2260,8 @@
       <c r="H26" t="s" s="2">
         <v>67</v>
       </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
     </row>
     <row r="27" ht="17" customHeight="1">
       <c r="A27" t="s" s="2">
@@ -2204,7 +2276,7 @@
       <c r="D27" t="s" s="2">
         <v>65</v>
       </c>
-      <c r="E27" t="s" s="3">
+      <c r="E27" t="s" s="4">
         <v>40</v>
       </c>
       <c r="F27" t="s" s="2">
@@ -2216,6 +2288,8 @@
       <c r="H27" t="s" s="2">
         <v>68</v>
       </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
     </row>
     <row r="28" ht="17" customHeight="1">
       <c r="A28" t="s" s="2">
@@ -2230,7 +2304,7 @@
       <c r="D28" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E28" t="s" s="3">
+      <c r="E28" t="s" s="4">
         <v>24</v>
       </c>
       <c r="F28" t="s" s="2">
@@ -2242,6 +2316,8 @@
       <c r="H28" t="s" s="2">
         <v>69</v>
       </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
     </row>
     <row r="29" ht="17" customHeight="1">
       <c r="A29" t="s" s="2">
@@ -2256,7 +2332,7 @@
       <c r="D29" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E29" t="s" s="3">
+      <c r="E29" t="s" s="4">
         <v>24</v>
       </c>
       <c r="F29" t="s" s="2">
@@ -2268,6 +2344,8 @@
       <c r="H29" t="s" s="2">
         <v>71</v>
       </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" ht="17" customHeight="1">
       <c r="A30" t="s" s="2">
@@ -2282,7 +2360,7 @@
       <c r="D30" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E30" t="s" s="3">
+      <c r="E30" t="s" s="4">
         <v>30</v>
       </c>
       <c r="F30" t="s" s="2">
@@ -2294,6 +2372,8 @@
       <c r="H30" t="s" s="2">
         <v>72</v>
       </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
     </row>
     <row r="31" ht="17" customHeight="1">
       <c r="A31" t="s" s="2">
@@ -2308,7 +2388,7 @@
       <c r="D31" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E31" t="s" s="3">
+      <c r="E31" t="s" s="4">
         <v>30</v>
       </c>
       <c r="F31" t="s" s="2">
@@ -2320,6 +2400,8 @@
       <c r="H31" t="s" s="2">
         <v>73</v>
       </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
     </row>
     <row r="32" ht="17" customHeight="1">
       <c r="A32" t="s" s="2">
@@ -2334,7 +2416,7 @@
       <c r="D32" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E32" t="s" s="3">
+      <c r="E32" t="s" s="4">
         <v>74</v>
       </c>
       <c r="F32" t="s" s="2">
@@ -2346,6 +2428,8 @@
       <c r="H32" t="s" s="2">
         <v>75</v>
       </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
     </row>
     <row r="33" ht="17" customHeight="1">
       <c r="A33" t="s" s="2">
@@ -2360,7 +2444,7 @@
       <c r="D33" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E33" t="s" s="3">
+      <c r="E33" t="s" s="4">
         <v>63</v>
       </c>
       <c r="F33" t="s" s="2">
@@ -2372,6 +2456,8 @@
       <c r="H33" t="s" s="2">
         <v>76</v>
       </c>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
     </row>
     <row r="34" ht="17" customHeight="1">
       <c r="A34" t="s" s="2">
@@ -2386,7 +2472,7 @@
       <c r="D34" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="E34" t="s" s="3">
+      <c r="E34" t="s" s="4">
         <v>63</v>
       </c>
       <c r="F34" t="s" s="2">
@@ -2398,6 +2484,8 @@
       <c r="H34" t="s" s="2">
         <v>77</v>
       </c>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
     </row>
     <row r="35" ht="17" customHeight="1">
       <c r="A35" t="s" s="2">
@@ -2412,7 +2500,7 @@
       <c r="D35" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="E35" t="s" s="3">
+      <c r="E35" t="s" s="4">
         <v>20</v>
       </c>
       <c r="F35" t="s" s="2">
@@ -2424,6 +2512,8 @@
       <c r="H35" t="s" s="2">
         <v>78</v>
       </c>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
     </row>
     <row r="36" ht="17" customHeight="1">
       <c r="A36" t="s" s="2">
@@ -2438,7 +2528,7 @@
       <c r="D36" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E36" t="s" s="3">
+      <c r="E36" t="s" s="4">
         <v>79</v>
       </c>
       <c r="F36" t="s" s="2">
@@ -2450,6 +2540,8 @@
       <c r="H36" t="s" s="2">
         <v>80</v>
       </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
     </row>
     <row r="37" ht="17" customHeight="1">
       <c r="A37" t="s" s="2">
@@ -2464,7 +2556,7 @@
       <c r="D37" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E37" t="s" s="3">
+      <c r="E37" t="s" s="4">
         <v>81</v>
       </c>
       <c r="F37" t="s" s="2">
@@ -2476,6 +2568,8 @@
       <c r="H37" t="s" s="2">
         <v>82</v>
       </c>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
     </row>
     <row r="38" ht="17" customHeight="1">
       <c r="A38" t="s" s="2">
@@ -2490,7 +2584,7 @@
       <c r="D38" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E38" t="s" s="3">
+      <c r="E38" t="s" s="4">
         <v>83</v>
       </c>
       <c r="F38" t="s" s="2">
@@ -2502,6 +2596,8 @@
       <c r="H38" t="s" s="2">
         <v>84</v>
       </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
     </row>
     <row r="39" ht="17" customHeight="1">
       <c r="A39" t="s" s="2">
@@ -2516,7 +2612,7 @@
       <c r="D39" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E39" t="s" s="3">
+      <c r="E39" t="s" s="4">
         <v>83</v>
       </c>
       <c r="F39" t="s" s="2">
@@ -2528,6 +2624,8 @@
       <c r="H39" t="s" s="2">
         <v>85</v>
       </c>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
     </row>
     <row r="40" ht="17" customHeight="1">
       <c r="A40" t="s" s="2">
@@ -2542,7 +2640,7 @@
       <c r="D40" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E40" t="s" s="3">
+      <c r="E40" t="s" s="4">
         <v>32</v>
       </c>
       <c r="F40" t="s" s="2">
@@ -2554,6 +2652,8 @@
       <c r="H40" t="s" s="2">
         <v>86</v>
       </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
     </row>
     <row r="41" ht="17" customHeight="1">
       <c r="A41" t="s" s="2">
@@ -2568,7 +2668,7 @@
       <c r="D41" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E41" t="s" s="3">
+      <c r="E41" t="s" s="4">
         <v>61</v>
       </c>
       <c r="F41" t="s" s="2">
@@ -2580,6 +2680,8 @@
       <c r="H41" t="s" s="2">
         <v>88</v>
       </c>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
     </row>
     <row r="42" ht="17" customHeight="1">
       <c r="A42" t="s" s="2">
@@ -2594,7 +2696,7 @@
       <c r="D42" t="s" s="2">
         <v>65</v>
       </c>
-      <c r="E42" t="s" s="3">
+      <c r="E42" t="s" s="4">
         <v>20</v>
       </c>
       <c r="F42" t="s" s="2">
@@ -2606,6 +2708,8 @@
       <c r="H42" t="s" s="2">
         <v>89</v>
       </c>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
     </row>
     <row r="43" ht="17" customHeight="1">
       <c r="A43" t="s" s="2">
@@ -2620,7 +2724,7 @@
       <c r="D43" t="s" s="2">
         <v>65</v>
       </c>
-      <c r="E43" t="s" s="3">
+      <c r="E43" t="s" s="4">
         <v>40</v>
       </c>
       <c r="F43" t="s" s="2">
@@ -2632,6 +2736,8 @@
       <c r="H43" t="s" s="2">
         <v>90</v>
       </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
     </row>
     <row r="44" ht="17" customHeight="1">
       <c r="A44" t="s" s="2">
@@ -2646,7 +2752,7 @@
       <c r="D44" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E44" t="s" s="3">
+      <c r="E44" t="s" s="4">
         <v>91</v>
       </c>
       <c r="F44" t="s" s="2">
@@ -2658,6 +2764,8 @@
       <c r="H44" t="s" s="2">
         <v>92</v>
       </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
     </row>
     <row r="45" ht="17" customHeight="1">
       <c r="A45" t="s" s="2">
@@ -2672,7 +2780,7 @@
       <c r="D45" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E45" t="s" s="3">
+      <c r="E45" t="s" s="4">
         <v>91</v>
       </c>
       <c r="F45" t="s" s="2">
@@ -2684,6 +2792,8 @@
       <c r="H45" t="s" s="2">
         <v>93</v>
       </c>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
     </row>
     <row r="46" ht="17" customHeight="1">
       <c r="A46" t="s" s="2">
@@ -2698,7 +2808,7 @@
       <c r="D46" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E46" t="s" s="3">
+      <c r="E46" t="s" s="4">
         <v>74</v>
       </c>
       <c r="F46" t="s" s="2">
@@ -2710,6 +2820,8 @@
       <c r="H46" t="s" s="2">
         <v>94</v>
       </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
     </row>
     <row r="47" ht="17" customHeight="1">
       <c r="A47" t="s" s="2">
@@ -2724,7 +2836,7 @@
       <c r="D47" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E47" t="s" s="3">
+      <c r="E47" t="s" s="4">
         <v>81</v>
       </c>
       <c r="F47" t="s" s="2">
@@ -2736,6 +2848,8 @@
       <c r="H47" t="s" s="2">
         <v>95</v>
       </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
     </row>
     <row r="48" ht="17" customHeight="1">
       <c r="A48" t="s" s="2">
@@ -2750,7 +2864,7 @@
       <c r="D48" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E48" t="s" s="3">
+      <c r="E48" t="s" s="4">
         <v>32</v>
       </c>
       <c r="F48" t="s" s="2">
@@ -2762,6 +2876,8 @@
       <c r="H48" t="s" s="2">
         <v>96</v>
       </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
     </row>
     <row r="49" ht="17" customHeight="1">
       <c r="A49" t="s" s="2">
@@ -2776,7 +2892,7 @@
       <c r="D49" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="E49" t="s" s="3">
+      <c r="E49" t="s" s="4">
         <v>98</v>
       </c>
       <c r="F49" t="s" s="2">
@@ -2788,6 +2904,8 @@
       <c r="H49" t="s" s="2">
         <v>99</v>
       </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
     </row>
     <row r="50" ht="17" customHeight="1">
       <c r="A50" t="s" s="2">
@@ -2802,7 +2920,7 @@
       <c r="D50" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E50" t="s" s="3">
+      <c r="E50" t="s" s="4">
         <v>30</v>
       </c>
       <c r="F50" t="s" s="2">
@@ -2814,6 +2932,8 @@
       <c r="H50" t="s" s="2">
         <v>100</v>
       </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
     </row>
     <row r="51" ht="17" customHeight="1">
       <c r="A51" t="s" s="2">
@@ -2828,7 +2948,7 @@
       <c r="D51" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="E51" t="s" s="3">
+      <c r="E51" t="s" s="4">
         <v>20</v>
       </c>
       <c r="F51" t="s" s="2">
@@ -2840,6 +2960,8 @@
       <c r="H51" t="s" s="2">
         <v>101</v>
       </c>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
     </row>
     <row r="52" ht="17" customHeight="1">
       <c r="A52" t="s" s="2">
@@ -2854,7 +2976,7 @@
       <c r="D52" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E52" t="s" s="3">
+      <c r="E52" t="s" s="4">
         <v>83</v>
       </c>
       <c r="F52" t="s" s="2">
@@ -2866,6 +2988,8 @@
       <c r="H52" t="s" s="2">
         <v>102</v>
       </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
     </row>
     <row r="53" ht="17" customHeight="1">
       <c r="A53" t="s" s="2">
@@ -2880,7 +3004,7 @@
       <c r="D53" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="E53" t="s" s="3">
+      <c r="E53" t="s" s="4">
         <v>74</v>
       </c>
       <c r="F53" t="s" s="2">
@@ -2892,6 +3016,8 @@
       <c r="H53" t="s" s="2">
         <v>103</v>
       </c>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
JinL - CCA data update
</commit_message>
<xml_diff>
--- a/data-transfer/transfer/data/cca/cca-class.xlsx
+++ b/data-transfer/transfer/data/cca/cca-class.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Class" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="110">
   <si>
     <t>Program</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Saturday</t>
   </si>
   <si>
-    <t>Thurday</t>
-  </si>
-  <si>
     <t>Sunday</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>B-Saturday-06</t>
   </si>
   <si>
-    <t>B-Thurday-05</t>
-  </si>
-  <si>
     <t>B-Thurday-01</t>
   </si>
   <si>
@@ -343,13 +337,25 @@
   </si>
   <si>
     <t>Clay-Sunday-01</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>B-Thurday-02</t>
+  </si>
+  <si>
+    <t>B-Friday-01</t>
+  </si>
+  <si>
+    <t>A-Sunday-03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -368,17 +374,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -435,18 +430,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="18" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1611,10 +1604,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV55"/>
+  <dimension ref="A1:IV57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H55"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1666,16 +1659,16 @@
       <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1694,16 +1687,16 @@
       <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1722,16 +1715,16 @@
       <c r="E4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1750,16 +1743,16 @@
       <c r="E5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="4"/>
+      <c r="G5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1778,16 +1771,16 @@
       <c r="E6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="4"/>
+      <c r="G6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1806,16 +1799,16 @@
       <c r="E7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="4"/>
+      <c r="G7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1834,16 +1827,16 @@
       <c r="E8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="4"/>
+      <c r="G8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1862,16 +1855,16 @@
       <c r="E9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="4"/>
+      <c r="G9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1890,16 +1883,16 @@
       <c r="E10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="4"/>
+      <c r="G10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1913,21 +1906,21 @@
         <v>8</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="4"/>
+      <c r="G11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1941,21 +1934,21 @@
         <v>21</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="4"/>
+      <c r="G12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1969,21 +1962,21 @@
         <v>11</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" s="4"/>
+      <c r="G13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1997,21 +1990,21 @@
         <v>8</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="I14" s="4"/>
+      <c r="G14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2025,21 +2018,21 @@
         <v>8</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="4"/>
+      <c r="G15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2053,21 +2046,21 @@
         <v>8</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I16" s="4"/>
+      <c r="G16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2081,21 +2074,21 @@
         <v>11</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I17" s="4"/>
+      <c r="G17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2109,32 +2102,32 @@
         <v>8</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I18" s="4"/>
+      <c r="G18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18"/>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>45</v>
@@ -2142,21 +2135,21 @@
       <c r="E19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I19" s="4"/>
+      <c r="G19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19"/>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>38</v>
@@ -2170,21 +2163,21 @@
       <c r="E20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" s="4"/>
+      <c r="G20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20"/>
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>38</v>
@@ -2198,21 +2191,21 @@
       <c r="E21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I21" s="4"/>
+      <c r="G21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21"/>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>38</v>
@@ -2226,21 +2219,21 @@
       <c r="E22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22" s="4"/>
+      <c r="G22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22"/>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>38</v>
@@ -2254,21 +2247,21 @@
       <c r="E23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="I23" s="4"/>
+      <c r="G23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23"/>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>38</v>
@@ -2277,54 +2270,54 @@
         <v>21</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="I24" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I24"/>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I25" s="4"/>
+      <c r="G25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25"/>
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>38</v>
@@ -2333,60 +2326,60 @@
         <v>11</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I26" s="4"/>
+      <c r="G26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I26"/>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="I27" s="4"/>
+      <c r="G27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27"/>
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>45</v>
@@ -2394,55 +2387,55 @@
       <c r="E28" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="I28" s="4"/>
+      <c r="G28" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28"/>
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G29" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="I29" s="4"/>
+      <c r="G29" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I29"/>
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>45</v>
@@ -2450,245 +2443,245 @@
       <c r="E30" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="I30" s="4"/>
+      <c r="G30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30"/>
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="I31" s="4"/>
+      <c r="G31" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31"/>
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="I32" s="4"/>
+      <c r="G32" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I32"/>
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I33" s="4"/>
+      <c r="G33" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I33"/>
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I34" s="4"/>
+      <c r="G34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I34"/>
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I35" s="4"/>
+      <c r="G35" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I35"/>
       <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G36" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I36" s="4"/>
+      <c r="G36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I36"/>
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F37" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G37" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="I37" s="4"/>
+      <c r="G37" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I37"/>
       <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F38" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I38" s="4"/>
+      <c r="G38" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I38"/>
       <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>38</v>
@@ -2697,200 +2690,200 @@
         <v>11</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G39" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="I39" s="4"/>
+      <c r="G39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I39"/>
       <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G40" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="I40" s="4"/>
+      <c r="G40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I40"/>
       <c r="J40" s="4"/>
     </row>
     <row r="41" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G41" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="I41" s="4"/>
+      <c r="G41" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I41"/>
       <c r="J41" s="4"/>
     </row>
     <row r="42" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F42" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="I42" s="4"/>
+      <c r="G42" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I42"/>
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="I43" s="4"/>
+      <c r="G43" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I43"/>
       <c r="J43" s="4"/>
     </row>
     <row r="44" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A44" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="I44" s="4"/>
+      <c r="G44" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I44"/>
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F45" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G45" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="I45" s="4"/>
+      <c r="G45" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I45"/>
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>45</v>
@@ -2898,161 +2891,161 @@
       <c r="E46" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G46" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I46" s="4"/>
+      <c r="G46" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I46"/>
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F47" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G47" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="I47" s="4"/>
+      <c r="G47" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I47"/>
       <c r="J47" s="4"/>
     </row>
     <row r="48" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F48" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G48" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H48" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="I48" s="4"/>
+      <c r="G48" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I48"/>
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G49" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I49" s="4"/>
+      <c r="G49" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I49"/>
       <c r="J49" s="4"/>
     </row>
     <row r="50" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I50" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I50"/>
       <c r="J50" s="4"/>
     </row>
     <row r="51" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="I51" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I51"/>
       <c r="J51" s="4"/>
     </row>
     <row r="52" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>38</v>
@@ -3061,26 +3054,26 @@
         <v>26</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G52" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I52" s="4"/>
+      <c r="G52" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I52"/>
       <c r="J52" s="4"/>
     </row>
     <row r="53" spans="1:10" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>38</v>
@@ -3089,26 +3082,26 @@
         <v>26</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F53" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G53" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="I53" s="4"/>
+      <c r="G53" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I53"/>
       <c r="J53" s="4"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1">
       <c r="A54" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>38</v>
@@ -3117,46 +3110,102 @@
         <v>26</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E54" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I54"/>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A55" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I55"/>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A56" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="F56" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G54" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A55" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C55" s="6" t="s">
+      <c r="G56" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I56"/>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A57" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E55" s="8" t="s">
+      <c r="D57" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F55" s="9" t="s">
+      <c r="F57" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G55" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>107</v>
-      </c>
+      <c r="G57" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I57"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
JinL - add tuition to data import, fix mobile login issue in imported data
</commit_message>
<xml_diff>
--- a/data-transfer/transfer/data/cca/cca-class.xlsx
+++ b/data-transfer/transfer/data/cca/cca-class.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="111">
   <si>
     <t>Program</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>A-Sunday-03</t>
+  </si>
+  <si>
+    <t>Tuition per class</t>
   </si>
 </sst>
 </file>
@@ -430,7 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -440,6 +443,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1607,7 +1611,7 @@
   <dimension ref="A1:IV57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1640,7 +1644,9 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4"/>
+      <c r="I1" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1668,7 +1674,9 @@
       <c r="H2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I2"/>
+      <c r="I2" s="9">
+        <v>25</v>
+      </c>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1696,7 +1704,9 @@
       <c r="H3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I3"/>
+      <c r="I3" s="9">
+        <v>25</v>
+      </c>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1724,7 +1734,9 @@
       <c r="H4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" s="9">
+        <v>25</v>
+      </c>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1752,7 +1764,9 @@
       <c r="H5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I5"/>
+      <c r="I5" s="9">
+        <v>25</v>
+      </c>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1780,7 +1794,9 @@
       <c r="H6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I6"/>
+      <c r="I6" s="9">
+        <v>25</v>
+      </c>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1808,7 +1824,9 @@
       <c r="H7" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I7"/>
+      <c r="I7" s="9">
+        <v>25</v>
+      </c>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1836,7 +1854,9 @@
       <c r="H8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I8"/>
+      <c r="I8" s="9">
+        <v>25</v>
+      </c>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1864,7 +1884,9 @@
       <c r="H9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I9"/>
+      <c r="I9" s="9">
+        <v>25</v>
+      </c>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1892,7 +1914,9 @@
       <c r="H10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I10"/>
+      <c r="I10" s="9">
+        <v>25</v>
+      </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1920,7 +1944,9 @@
       <c r="H11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I11"/>
+      <c r="I11" s="9">
+        <v>25</v>
+      </c>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1948,7 +1974,9 @@
       <c r="H12" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="I12"/>
+      <c r="I12" s="9">
+        <v>25</v>
+      </c>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -1976,7 +2004,9 @@
       <c r="H13" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I13"/>
+      <c r="I13" s="9">
+        <v>25</v>
+      </c>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2004,7 +2034,9 @@
       <c r="H14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I14"/>
+      <c r="I14" s="9">
+        <v>25</v>
+      </c>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2032,7 +2064,9 @@
       <c r="H15" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I15"/>
+      <c r="I15" s="9">
+        <v>25</v>
+      </c>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2060,7 +2094,9 @@
       <c r="H16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I16"/>
+      <c r="I16" s="9">
+        <v>25</v>
+      </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2088,7 +2124,9 @@
       <c r="H17" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I17"/>
+      <c r="I17" s="9">
+        <v>25</v>
+      </c>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2116,7 +2154,9 @@
       <c r="H18" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I18"/>
+      <c r="I18" s="9">
+        <v>25</v>
+      </c>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2144,7 +2184,9 @@
       <c r="H19" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I19"/>
+      <c r="I19" s="9">
+        <v>25</v>
+      </c>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2172,7 +2214,9 @@
       <c r="H20" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I20"/>
+      <c r="I20" s="9">
+        <v>40</v>
+      </c>
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2200,7 +2244,9 @@
       <c r="H21" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I21"/>
+      <c r="I21" s="9">
+        <v>30</v>
+      </c>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2228,7 +2274,9 @@
       <c r="H22" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I22"/>
+      <c r="I22" s="9">
+        <v>30</v>
+      </c>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2256,7 +2304,9 @@
       <c r="H23" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I23"/>
+      <c r="I23" s="9">
+        <v>30</v>
+      </c>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2284,7 +2334,9 @@
       <c r="H24" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I24"/>
+      <c r="I24" s="9">
+        <v>30</v>
+      </c>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2312,7 +2364,9 @@
       <c r="H25" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="I25"/>
+      <c r="I25" s="9">
+        <v>30</v>
+      </c>
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2340,7 +2394,9 @@
       <c r="H26" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="I26"/>
+      <c r="I26" s="9">
+        <v>30</v>
+      </c>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2368,7 +2424,9 @@
       <c r="H27" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I27"/>
+      <c r="I27" s="9">
+        <v>30</v>
+      </c>
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2396,7 +2454,9 @@
       <c r="H28" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="I28"/>
+      <c r="I28" s="9">
+        <v>30</v>
+      </c>
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2424,7 +2484,9 @@
       <c r="H29" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="I29"/>
+      <c r="I29" s="9">
+        <v>30</v>
+      </c>
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2452,7 +2514,9 @@
       <c r="H30" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I30"/>
+      <c r="I30" s="9">
+        <v>30</v>
+      </c>
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2480,7 +2544,9 @@
       <c r="H31" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="I31"/>
+      <c r="I31" s="9">
+        <v>30</v>
+      </c>
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2508,7 +2574,9 @@
       <c r="H32" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I32"/>
+      <c r="I32" s="9">
+        <v>30</v>
+      </c>
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2536,7 +2604,9 @@
       <c r="H33" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="I33"/>
+      <c r="I33" s="9">
+        <v>30</v>
+      </c>
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2564,7 +2634,9 @@
       <c r="H34" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I34"/>
+      <c r="I34" s="9">
+        <v>30</v>
+      </c>
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2592,7 +2664,9 @@
       <c r="H35" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="I35"/>
+      <c r="I35" s="9">
+        <v>30</v>
+      </c>
       <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2620,7 +2694,9 @@
       <c r="H36" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="I36"/>
+      <c r="I36" s="9">
+        <v>30</v>
+      </c>
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2648,7 +2724,9 @@
       <c r="H37" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I37"/>
+      <c r="I37" s="9">
+        <v>30</v>
+      </c>
       <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2676,7 +2754,9 @@
       <c r="H38" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="I38"/>
+      <c r="I38" s="9">
+        <v>30</v>
+      </c>
       <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2704,7 +2784,9 @@
       <c r="H39" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I39"/>
+      <c r="I39" s="9">
+        <v>30</v>
+      </c>
       <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2732,7 +2814,9 @@
       <c r="H40" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="I40"/>
+      <c r="I40" s="9">
+        <v>30</v>
+      </c>
       <c r="J40" s="4"/>
     </row>
     <row r="41" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2760,7 +2844,9 @@
       <c r="H41" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="I41"/>
+      <c r="I41" s="9">
+        <v>30</v>
+      </c>
       <c r="J41" s="4"/>
     </row>
     <row r="42" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2788,7 +2874,9 @@
       <c r="H42" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="I42"/>
+      <c r="I42" s="9">
+        <v>30</v>
+      </c>
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2816,7 +2904,9 @@
       <c r="H43" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I43"/>
+      <c r="I43" s="9">
+        <v>30</v>
+      </c>
       <c r="J43" s="4"/>
     </row>
     <row r="44" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2844,7 +2934,9 @@
       <c r="H44" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="I44"/>
+      <c r="I44" s="9">
+        <v>30</v>
+      </c>
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2872,7 +2964,9 @@
       <c r="H45" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="I45"/>
+      <c r="I45" s="9">
+        <v>30</v>
+      </c>
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2900,7 +2994,9 @@
       <c r="H46" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="I46"/>
+      <c r="I46" s="9">
+        <v>30</v>
+      </c>
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2928,7 +3024,9 @@
       <c r="H47" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="I47"/>
+      <c r="I47" s="9">
+        <v>30</v>
+      </c>
       <c r="J47" s="4"/>
     </row>
     <row r="48" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2956,7 +3054,9 @@
       <c r="H48" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I48"/>
+      <c r="I48" s="9">
+        <v>30</v>
+      </c>
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -2984,7 +3084,9 @@
       <c r="H49" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I49"/>
+      <c r="I49" s="9">
+        <v>30</v>
+      </c>
       <c r="J49" s="4"/>
     </row>
     <row r="50" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -3012,7 +3114,9 @@
       <c r="H50" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I50"/>
+      <c r="I50" s="9">
+        <v>30</v>
+      </c>
       <c r="J50" s="4"/>
     </row>
     <row r="51" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -3040,7 +3144,9 @@
       <c r="H51" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="I51"/>
+      <c r="I51" s="9">
+        <v>30</v>
+      </c>
       <c r="J51" s="4"/>
     </row>
     <row r="52" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -3068,7 +3174,9 @@
       <c r="H52" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="I52"/>
+      <c r="I52" s="9">
+        <v>40</v>
+      </c>
       <c r="J52" s="4"/>
     </row>
     <row r="53" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -3096,7 +3204,9 @@
       <c r="H53" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="I53"/>
+      <c r="I53" s="9">
+        <v>40</v>
+      </c>
       <c r="J53" s="4"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1">
@@ -3124,7 +3234,9 @@
       <c r="H54" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I54"/>
+      <c r="I54" s="9">
+        <v>40</v>
+      </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" customHeight="1">
       <c r="A55" s="6" t="s">
@@ -3151,7 +3263,9 @@
       <c r="H55" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="I55"/>
+      <c r="I55" s="9">
+        <v>40</v>
+      </c>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1">
       <c r="A56" s="6" t="s">
@@ -3178,7 +3292,9 @@
       <c r="H56" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I56"/>
+      <c r="I56" s="9">
+        <v>40</v>
+      </c>
     </row>
     <row r="57" spans="1:10" ht="15.75" customHeight="1">
       <c r="A57" s="7" t="s">
@@ -3205,7 +3321,9 @@
       <c r="H57" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="I57"/>
+      <c r="I57" s="9">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>